<commit_message>
Added validations for Car on TripFolderPage
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/HotelScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/HotelScenarios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Description</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Registered</t>
+  </si>
+  <si>
+    <t>Holiday Inn Club Vacations LAS VEGAS</t>
   </si>
 </sst>
 </file>
@@ -283,6 +286,17 @@
   </cellStyles>
   <dxfs count="20">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -295,17 +309,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -615,8 +618,8 @@
     <tableColumn id="10" name="StarRating" dataDxfId="4"/>
     <tableColumn id="11" name="Supplier" dataDxfId="3"/>
     <tableColumn id="14" name="PostSearchFilters" dataDxfId="2"/>
-    <tableColumn id="2" name="UserType" dataDxfId="0"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="1"/>
+    <tableColumn id="2" name="UserType" dataDxfId="1"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -914,7 +917,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="N13" sqref="N13"/>
+      <selection pane="topRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1011,9 @@
         <v>16</v>
       </c>
       <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="K2" s="5"/>
       <c r="L2" s="6" t="s">
         <v>22</v>

</xml_diff>